<commit_message>
Refactory and include another way to create a job
</commit_message>
<xml_diff>
--- a/Data/problem_data.xlsx
+++ b/Data/problem_data.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="machines" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="work types" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="supplier order" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="customer order" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="customer deadlines" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -653,85 +652,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>id_work_type</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>quantity</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>W0</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>W1</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>W2</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>W3</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>W4</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>